<commit_message>
Versão bootstrap com estilo ok
</commit_message>
<xml_diff>
--- a/modelo_dados.xlsx
+++ b/modelo_dados.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VENDAS\Projeto_aproverba_bkp\aproverba\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jefferson\Projetos\aproverba\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E08641A-9391-4C52-9007-256F6E491164}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A05171A-2118-46D2-8A99-1AAC4C3F9EE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="verba" sheetId="4" r:id="rId1"/>
@@ -19,6 +19,9 @@
     <sheet name="fluxo" sheetId="3" r:id="rId4"/>
     <sheet name="fila" sheetId="6" r:id="rId5"/>
     <sheet name="inf_etapas" sheetId="5" r:id="rId6"/>
+    <sheet name="menu" sheetId="7" r:id="rId7"/>
+    <sheet name="tela_relatorios" sheetId="9" r:id="rId8"/>
+    <sheet name="tela_Acomp_oc" sheetId="8" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -153,7 +156,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="129">
   <si>
     <t>codigo</t>
   </si>
@@ -483,6 +486,63 @@
   </si>
   <si>
     <t>e uma etapa para conferencia</t>
+  </si>
+  <si>
+    <t>Lançamentos</t>
+  </si>
+  <si>
+    <t>Verbas</t>
+  </si>
+  <si>
+    <t>Pedidos de compra</t>
+  </si>
+  <si>
+    <t>Diretoria/Aprovação</t>
+  </si>
+  <si>
+    <t>Fiscal</t>
+  </si>
+  <si>
+    <t>Análises PCs</t>
+  </si>
+  <si>
+    <t>Acompanhamentos OCs</t>
+  </si>
+  <si>
+    <t>Abertas</t>
+  </si>
+  <si>
+    <t>Análise</t>
+  </si>
+  <si>
+    <t>Negada/Cancelada</t>
+  </si>
+  <si>
+    <t>Liberadas</t>
+  </si>
+  <si>
+    <t>Filtro</t>
+  </si>
+  <si>
+    <t>Relatórios</t>
+  </si>
+  <si>
+    <t>criar um painel com vários quadros de informações, com tabelas e gráficos</t>
+  </si>
+  <si>
+    <t>definir os indicadores e visuais</t>
+  </si>
+  <si>
+    <t>Sobre/Ajuda</t>
+  </si>
+  <si>
+    <t>Logout</t>
+  </si>
+  <si>
+    <t>Usuário</t>
+  </si>
+  <si>
+    <t>Login</t>
   </si>
 </sst>
 </file>
@@ -1620,7 +1680,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99A67273-8300-422E-8516-9941FD29AA5A}">
   <dimension ref="A1:B42"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A23" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
@@ -1815,4 +1875,138 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7853C420-4622-430F-BC23-9FA1DF15D116}">
+  <dimension ref="A1:H4"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="H1" s="4"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B2" t="s">
+        <v>113</v>
+      </c>
+      <c r="G2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B3" t="s">
+        <v>114</v>
+      </c>
+      <c r="G3" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4394C4E4-5687-496E-969E-4CD885819D2B}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05DBAB34-0EDE-4ACD-88FC-5CF467495A13}">
+  <dimension ref="A1:A5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>120</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>